<commit_message>
Finished Code Category module
</commit_message>
<xml_diff>
--- a/Spring/shopme-commerce-project/sample-data/Shopme Sample Users Data.xlsx
+++ b/Spring/shopme-commerce-project/sample-data/Shopme Sample Users Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Spring\Personal-Projects\Spring\shopme-commerce-project\sample-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DFD483-35A8-4352-A4B3-C185EF39D699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E9D090-AED5-44EA-B4C7-51B3E71AED94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -530,10 +530,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -833,10 +833,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -920,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -936,14 +936,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -975,7 +975,7 @@
       <c r="A5" s="3">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1287,7 +1287,7 @@
       <c r="A17" s="3">
         <v>13</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -1578,6 +1578,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B17" r:id="rId1" xr:uid="{5C2E503C-B073-4BAA-B990-6A3BB6CDE445}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{D990DAC0-66C1-47CB-9067-5C319D11EFE8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>